<commit_message>
added amoung and income to fake data 2021 and 2020
</commit_message>
<xml_diff>
--- a/data-raw/FAKE_DATA_2020.xlsx
+++ b/data-raw/FAKE_DATA_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flhug/Dropbox (Personal)/PhD/Courses/H4Sci_Project/Git/pseudonymizer/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A6ED0C-4AA6-B746-A16C-4D0753D45790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA06F72-1928-E645-B526-F40269D254E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="-9660" windowWidth="38400" windowHeight="23500" xr2:uid="{F2FEE1B5-A181-9D49-99C5-546F0817DC33}"/>
+    <workbookView xWindow="25600" yWindow="8560" windowWidth="38400" windowHeight="10560" xr2:uid="{F2FEE1B5-A181-9D49-99C5-546F0817DC33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>NNSS</t>
   </si>
@@ -144,6 +144,18 @@
   </si>
   <si>
     <t>Eichenweg</t>
+  </si>
+  <si>
+    <t>EGID</t>
+  </si>
+  <si>
+    <t>EWID</t>
+  </si>
+  <si>
+    <t>AMOUNT</t>
+  </si>
+  <si>
+    <t>STEUERBARESEINKOMMEN</t>
   </si>
 </sst>
 </file>
@@ -514,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91BF7B3D-EBD7-8C4D-A454-F3444C20C8ED}">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:K3"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -531,7 +543,7 @@
     <col min="10" max="11" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -572,16 +584,28 @@
         <v>10</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="T1" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:20">
       <c r="A2" s="3">
         <v>7560000000001</v>
       </c>
@@ -622,16 +646,28 @@
         <v>20</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>222</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P2">
         <v>0</v>
       </c>
+      <c r="Q2">
+        <v>25000</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>-100</v>
+      </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:20">
       <c r="A3" s="3">
         <v>7560000000004</v>
       </c>
@@ -669,16 +705,28 @@
         <v>30</v>
       </c>
       <c r="N3">
+        <v>1231</v>
+      </c>
+      <c r="O3">
+        <v>122</v>
+      </c>
+      <c r="P3">
         <v>10000</v>
       </c>
-      <c r="O3">
+      <c r="Q3">
+        <v>500000</v>
+      </c>
+      <c r="R3">
         <v>1</v>
       </c>
-      <c r="P3">
+      <c r="S3">
         <v>0</v>
       </c>
+      <c r="T3">
+        <v>777</v>
+      </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:20">
       <c r="A4" s="3">
         <v>7560000000005</v>
       </c>
@@ -715,8 +763,20 @@
       <c r="M4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="5">
+        <v>9999999</v>
+      </c>
+      <c r="O4" s="5">
+        <v>999</v>
+      </c>
+      <c r="P4">
         <v>20000</v>
+      </c>
+      <c r="Q4">
+        <v>50000</v>
+      </c>
+      <c r="T4">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>